<commit_message>
modified text in requirements doc
</commit_message>
<xml_diff>
--- a/tcl3-data-apis/files/requirements_table.xlsx
+++ b/tcl3-data-apis/files/requirements_table.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akishiha/git_repos/utm-apis/tcl3-data-apis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akishiha/git_repos/utm-apis/tcl3-data-apis/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{9D3E1166-B257-164E-87C0-96D137748927}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="560" windowWidth="27640" windowHeight="16240"/>
+    <workbookView xWindow="780" yWindow="460" windowWidth="27640" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -128,9 +129,6 @@
     <t>x</t>
   </si>
   <si>
-    <t>UTM-TCL3-DMP-RevF-SAAPDF</t>
-  </si>
-  <si>
     <t>CONPDF</t>
   </si>
   <si>
@@ -144,12 +142,15 @@
   </si>
   <si>
     <t>DAT5</t>
+  </si>
+  <si>
+    <t>SAAPDF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -503,11 +504,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -520,7 +521,7 @@
     <col min="41" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="80" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -537,7 +538,7 @@
         <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>6</v>
@@ -560,8 +561,8 @@
       <c r="M1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>34</v>
+      <c r="N1" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>26</v>
@@ -579,10 +580,10 @@
         <v>32</v>
       </c>
       <c r="T1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="U1" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="V1" s="2" t="s">
         <v>27</v>
@@ -591,10 +592,10 @@
         <v>28</v>
       </c>
       <c r="X1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y1" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
@@ -793,7 +794,7 @@
     </row>
     <row r="18" spans="1:25" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="X18" s="2" t="s">
         <v>33</v>
@@ -801,7 +802,7 @@
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Y19" s="2" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
updated requirements table - add flight_data to DAT4 since we need to know vehicle data to compute the distance form the uas_id observer to the vehicle during the lookup tests
</commit_message>
<xml_diff>
--- a/tcl3-data-apis/files/requirements_table.xlsx
+++ b/tcl3-data-apis/files/requirements_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akishiha/git_repos/utm-apis/tcl3-data-apis/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{9D3E1166-B257-164E-87C0-96D137748927}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{86780FBD-D7C9-6048-B82F-5656A3BC8CEC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="460" windowWidth="27640" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="40">
   <si>
     <t>Test Identifier</t>
   </si>
@@ -508,7 +508,7 @@
   <dimension ref="A1:AN19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -780,6 +780,9 @@
       <c r="A16" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="B16" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="V16" s="2" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
updated yaml files; removed the string lists and replace with object arrays
</commit_message>
<xml_diff>
--- a/tcl3-data-apis/files/requirements_table.xlsx
+++ b/tcl3-data-apis/files/requirements_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akishiha/git_repos/utm-apis/tcl3-data-apis/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{86780FBD-D7C9-6048-B82F-5656A3BC8CEC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{9C73EB80-60EC-5249-A6E3-610BE048DFDC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="460" windowWidth="27640" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7320" yWindow="1860" windowWidth="27640" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -505,10 +505,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:AN19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -812,7 +815,8 @@
       </c>
     </row>
   </sheetData>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup scale="49" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated requirements table - correct error in CON1
</commit_message>
<xml_diff>
--- a/tcl3-data-apis/files/requirements_table.xlsx
+++ b/tcl3-data-apis/files/requirements_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akishiha/git_repos/utm-apis/tcl3-data-apis/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eotorres/Documents/TCL3-2018_National_Campaign/DMP/OfficialUTM-Github-utm-apis-files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{9C73EB80-60EC-5249-A6E3-610BE048DFDC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{92F9B83E-33E3-7548-9242-CAD6AB471A3C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7320" yWindow="1860" windowWidth="27640" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29520" yWindow="4820" windowWidth="33700" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="40">
   <si>
     <t>Test Identifier</t>
   </si>
@@ -511,15 +511,34 @@
   <dimension ref="A1:AN19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="2" customWidth="1"/>
-    <col min="3" max="23" width="9" style="2" customWidth="1"/>
-    <col min="24" max="39" width="10.83203125" style="2"/>
+    <col min="3" max="3" width="11.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="12" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="8.5" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" style="2" customWidth="1"/>
+    <col min="8" max="9" width="11.83203125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="11.1640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="11.5" style="2" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="9" style="2" customWidth="1"/>
+    <col min="15" max="15" width="11.1640625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="11.5" style="2" customWidth="1"/>
+    <col min="17" max="17" width="10.5" style="2" customWidth="1"/>
+    <col min="18" max="19" width="10.83203125" style="2" customWidth="1"/>
+    <col min="20" max="21" width="9" style="2" customWidth="1"/>
+    <col min="22" max="22" width="6.5" style="2" customWidth="1"/>
+    <col min="23" max="23" width="8" style="2" customWidth="1"/>
+    <col min="24" max="24" width="10.83203125" style="2"/>
+    <col min="25" max="25" width="6.6640625" style="2" customWidth="1"/>
+    <col min="26" max="39" width="10.83203125" style="2"/>
     <col min="40" max="40" width="10.83203125" style="3"/>
     <col min="41" max="16384" width="10.83203125" style="1"/>
   </cols>
@@ -725,6 +744,9 @@
       <c r="O11" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="T11" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">

</xml_diff>